<commit_message>
feat(PYME-3909): Add system column in each row
</commit_message>
<xml_diff>
--- a/reports/request_type_status_report/templates/xlsx/template.xlsx
+++ b/reports/request_type_status_report/templates/xlsx/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/lastest_subscriptions_changes/templates/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/request_type_status_report/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F93526-1C31-324D-8F39-D0492B71F233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A22A92-1488-134D-9395-543D59AD18BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>CIF</t>
   </si>
@@ -384,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:M1048576"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -397,9 +397,10 @@
     <col min="3" max="3" width="19.6640625" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="17.5" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,9 +416,12 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(PYME-3909): Add system column in each row (#20)
* feat(PYME-3909): Add system column in each row

* Create constant
</commit_message>
<xml_diff>
--- a/reports/request_type_status_report/templates/xlsx/template.xlsx
+++ b/reports/request_type_status_report/templates/xlsx/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/lastest_subscriptions_changes/templates/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/request_type_status_report/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F93526-1C31-324D-8F39-D0492B71F233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09659639-8068-D04A-A10A-D94CF7EB93EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>CIF</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>OPERACIÓN</t>
+  </si>
+  <si>
+    <t>SISTEMA</t>
   </si>
 </sst>
 </file>
@@ -384,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:M1048576"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -397,9 +400,10 @@
     <col min="3" max="3" width="19.6640625" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="17.5" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,9 +419,12 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Include change in Request type and status reportt
</commit_message>
<xml_diff>
--- a/reports/request_type_status_report/templates/xlsx/template.xlsx
+++ b/reports/request_type_status_report/templates/xlsx/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/request_type_status_report/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09659639-8068-D04A-A10A-D94CF7EB93EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA158D98-7390-284C-8835-346D158D9142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>CIF</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>SISTEMA</t>
+  </si>
+  <si>
+    <t>SUBSCRIPCIÓN</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -399,11 +402,11 @@
     <col min="2" max="2" width="22" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="5" max="6" width="17.5" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -422,9 +425,12 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feat/pyme 6029 implement subscription name for new products (#35)
* feat(PYME-6029): Implement new Subscription name for new package

* Include change in Request type and status reportt

* Fix code review changes

* Fix code review changes requested
</commit_message>
<xml_diff>
--- a/reports/request_type_status_report/templates/xlsx/template.xlsx
+++ b/reports/request_type_status_report/templates/xlsx/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/request_type_status_report/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09659639-8068-D04A-A10A-D94CF7EB93EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA158D98-7390-284C-8835-346D158D9142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>CIF</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>SISTEMA</t>
+  </si>
+  <si>
+    <t>SUBSCRIPCIÓN</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -399,11 +402,11 @@
     <col min="2" max="2" width="22" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="5" max="6" width="17.5" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -422,9 +425,12 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>